<commit_message>
Restructured code to try to get imports correct so that unit tests can run
</commit_message>
<xml_diff>
--- a/tests/Test_plates/Test_plate_1_repeat_1.xlsx
+++ b/tests/Test_plates/Test_plate_1_repeat_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ks17361/Lab_work_Dek_Woolfson/BADASS/sensing_array_paper_2019/tests/Test_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30D8658-6D5D-AF4B-BCCD-9EFFE5FB9FDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B51CA6-224D-2F48-803E-5A42A6F19E5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="2440" windowWidth="27300" windowHeight="14240" xr2:uid="{3108E363-480C-1C4C-B971-293712F19C9B}"/>
   </bookViews>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E78E01-51D6-624A-8582-548840E6FF26}">
   <dimension ref="A3:Y77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G36" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2918,7 +2918,7 @@
         <v>0.53265323916644869</v>
       </c>
       <c r="I62">
-        <f t="shared" si="14"/>
+        <f xml:space="preserve"> (Q20 - $B$40) / (I50 - $B$40)</f>
         <v>0.51751059558331469</v>
       </c>
       <c r="J62">
@@ -2979,7 +2979,7 @@
         <v>0.51460458627604844</v>
       </c>
       <c r="I63">
-        <f t="shared" si="16"/>
+        <f xml:space="preserve"> (Y18 - $B$40) / (I50 - $B$40)</f>
         <v>0.50992638857907646</v>
       </c>
       <c r="J63">
@@ -3040,7 +3040,7 @@
         <v>0.52358531694132004</v>
       </c>
       <c r="I64">
-        <f t="shared" si="18"/>
+        <f xml:space="preserve"> (Y20 - $B$40) / (I50 - $B$40)</f>
         <v>0.56078518848985059</v>
       </c>
       <c r="J64">
@@ -3101,7 +3101,7 @@
         <v>0.52803208649402733</v>
       </c>
       <c r="I65">
-        <f t="shared" si="20"/>
+        <f xml:space="preserve"> (Y28 - $B$40) / (I50 - $B$40)</f>
         <v>0.53714030782957845</v>
       </c>
       <c r="J65">

</xml_diff>